<commit_message>
commit all project alami sharia
</commit_message>
<xml_diff>
--- a/Data/DataAlamiSharia.xlsx
+++ b/Data/DataAlamiSharia.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Registrasi" sheetId="1" r:id="rId1"/>
-    <sheet name="Login" sheetId="2" r:id="rId2"/>
+    <sheet name="Verifikasi" sheetId="3" r:id="rId2"/>
+    <sheet name="Login" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -86,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="68">
   <si>
     <t>email</t>
   </si>
@@ -134,6 +135,162 @@
   </si>
   <si>
     <t>test2@yopmail.com</t>
+  </si>
+  <si>
+    <t>tipeAkun</t>
+  </si>
+  <si>
+    <t>gelar</t>
+  </si>
+  <si>
+    <t>jenisKelamin</t>
+  </si>
+  <si>
+    <t>tempatLahir</t>
+  </si>
+  <si>
+    <t>agama</t>
+  </si>
+  <si>
+    <t>namaIbuKandung</t>
+  </si>
+  <si>
+    <t>statusPernikahan</t>
+  </si>
+  <si>
+    <t>pendidikanTerakhir</t>
+  </si>
+  <si>
+    <t>alamat</t>
+  </si>
+  <si>
+    <t>rt</t>
+  </si>
+  <si>
+    <t>rw</t>
+  </si>
+  <si>
+    <t>kabKota</t>
+  </si>
+  <si>
+    <t>kecamatan</t>
+  </si>
+  <si>
+    <t>kelurahan</t>
+  </si>
+  <si>
+    <t>pekerjaan</t>
+  </si>
+  <si>
+    <t>bidangPekerjaan</t>
+  </si>
+  <si>
+    <t>penghasilanBulanan</t>
+  </si>
+  <si>
+    <t>sumberDana</t>
+  </si>
+  <si>
+    <t>namakontakDarurat</t>
+  </si>
+  <si>
+    <t>noHandphoneKontakDarurat</t>
+  </si>
+  <si>
+    <t>nomorKTP</t>
+  </si>
+  <si>
+    <t>kotaPenerbitKTP</t>
+  </si>
+  <si>
+    <t>nomorNPWP</t>
+  </si>
+  <si>
+    <t>uploadKTP</t>
+  </si>
+  <si>
+    <t>uploadNPWP</t>
+  </si>
+  <si>
+    <t>namaBank</t>
+  </si>
+  <si>
+    <t>nomorRekening</t>
+  </si>
+  <si>
+    <t>rofiimron@gmail.com</t>
+  </si>
+  <si>
+    <t>Individual - WNI (Mewakili Diri Sendiri)</t>
+  </si>
+  <si>
+    <t>Bpk</t>
+  </si>
+  <si>
+    <t>Imron</t>
+  </si>
+  <si>
+    <t>Laki-laki</t>
+  </si>
+  <si>
+    <t>859859859859</t>
+  </si>
+  <si>
+    <t>Kota Malang</t>
+  </si>
+  <si>
+    <t>Islam</t>
+  </si>
+  <si>
+    <t>Umi</t>
+  </si>
+  <si>
+    <t>Menikah</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>jl sampurna no.32 B</t>
+  </si>
+  <si>
+    <t>Kedungkandang</t>
+  </si>
+  <si>
+    <t>Cemorokandang</t>
+  </si>
+  <si>
+    <t>Pegawai Swasta</t>
+  </si>
+  <si>
+    <t>Informasi dan Komunikasi</t>
+  </si>
+  <si>
+    <t>10 - 20 juta rupiah</t>
+  </si>
+  <si>
+    <t>Gaji</t>
+  </si>
+  <si>
+    <t>Aulina</t>
+  </si>
+  <si>
+    <t>6549875454165589</t>
+  </si>
+  <si>
+    <t>852852852852</t>
+  </si>
+  <si>
+    <t>123654785424554</t>
+  </si>
+  <si>
+    <t>ktp</t>
+  </si>
+  <si>
+    <t>npwp</t>
+  </si>
+  <si>
+    <t>BANK BCA SYARIAH</t>
   </si>
 </sst>
 </file>
@@ -478,7 +635,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
@@ -553,6 +710,242 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AE2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="S29" sqref="S29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="15.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>28</v>
+      </c>
+      <c r="R1" t="s">
+        <v>29</v>
+      </c>
+      <c r="S1" t="s">
+        <v>30</v>
+      </c>
+      <c r="T1" t="s">
+        <v>31</v>
+      </c>
+      <c r="U1" t="s">
+        <v>32</v>
+      </c>
+      <c r="V1" t="s">
+        <v>33</v>
+      </c>
+      <c r="W1" t="s">
+        <v>34</v>
+      </c>
+      <c r="X1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I2" t="s">
+        <v>50</v>
+      </c>
+      <c r="J2" t="s">
+        <v>51</v>
+      </c>
+      <c r="K2" t="s">
+        <v>52</v>
+      </c>
+      <c r="L2" t="s">
+        <v>53</v>
+      </c>
+      <c r="M2" t="s">
+        <v>54</v>
+      </c>
+      <c r="N2">
+        <v>3</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>55</v>
+      </c>
+      <c r="R2" t="s">
+        <v>56</v>
+      </c>
+      <c r="S2" t="s">
+        <v>57</v>
+      </c>
+      <c r="T2" t="s">
+        <v>58</v>
+      </c>
+      <c r="U2" t="s">
+        <v>59</v>
+      </c>
+      <c r="V2" t="s">
+        <v>60</v>
+      </c>
+      <c r="W2" t="s">
+        <v>61</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE2">
+        <v>312456897</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>